<commit_message>
Nu har jag lagt till bilder och text. Kolla igenon du också.
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dropbox\Databasteknik\Hemsida\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{822F0B5B-76B9-4EFE-9AAF-9B0D2B16E223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92556CA-DA22-49CF-AAB7-5E89D5DE05A7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1500" windowWidth="29040" windowHeight="15840" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
+    <workbookView xWindow="-19320" yWindow="765" windowWidth="19440" windowHeight="15000" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
   <si>
     <t>Uppgift</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Produktlänkar från databasen</t>
   </si>
   <si>
-    <t>Hämta produkter från databasen och genera klickbara länkar till produkterna.</t>
-  </si>
-  <si>
     <t>Produktkategorier</t>
   </si>
   <si>
@@ -139,13 +136,25 @@
   </si>
   <si>
     <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>I menyn bestäms kategorier och länkar till produkterna av det som finns i databasen.</t>
+  </si>
+  <si>
+    <t>Front end/databas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,13 +177,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
@@ -183,7 +185,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,13 +202,8 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -321,34 +318,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Bra" xfId="1" builtinId="26"/>
     <cellStyle name="Dålig" xfId="2" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -663,13 +670,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18B0A93-A15E-478B-B68F-0A6D7C63864A}">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
@@ -680,7 +687,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -718,8 +725,8 @@
         <v>6</v>
       </c>
       <c r="E2" s="7"/>
-      <c r="F2" s="6" t="s">
-        <v>36</v>
+      <c r="F2" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="G2" s="8"/>
       <c r="J2" t="s">
@@ -740,8 +747,8 @@
         <v>6</v>
       </c>
       <c r="E3" s="7"/>
-      <c r="F3" s="6" t="s">
-        <v>36</v>
+      <c r="F3" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="G3" s="8"/>
       <c r="J3" t="s">
@@ -762,8 +769,8 @@
         <v>6</v>
       </c>
       <c r="E4" s="7"/>
-      <c r="F4" s="6" t="s">
-        <v>36</v>
+      <c r="F4" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="G4" s="8"/>
     </row>
@@ -781,8 +788,8 @@
         <v>14</v>
       </c>
       <c r="E5" s="7"/>
-      <c r="F5" s="6" t="s">
-        <v>36</v>
+      <c r="F5" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="G5" s="8"/>
     </row>
@@ -800,8 +807,8 @@
         <v>17</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="6" t="s">
-        <v>36</v>
+      <c r="F6" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="G6" s="8"/>
     </row>
@@ -819,8 +826,8 @@
         <v>14</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="6" t="s">
-        <v>36</v>
+      <c r="F7" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="G7" s="8"/>
     </row>
@@ -838,8 +845,8 @@
         <v>6</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="6" t="s">
-        <v>37</v>
+      <c r="F8" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="G8" s="8"/>
     </row>
@@ -851,14 +858,14 @@
         <v>12</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="7"/>
-      <c r="F9" s="6" t="s">
-        <v>37</v>
+      <c r="F9" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="G9" s="8"/>
     </row>
@@ -876,8 +883,8 @@
         <v>17</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="6" t="s">
-        <v>37</v>
+      <c r="F10" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="G10" s="8"/>
     </row>
@@ -889,14 +896,14 @@
         <v>22</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="6" t="s">
-        <v>37</v>
+      <c r="F11" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="G11" s="8"/>
     </row>
@@ -914,8 +921,8 @@
         <v>14</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="6" t="s">
-        <v>37</v>
+      <c r="F12" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="G12" s="8"/>
     </row>
@@ -924,35 +931,37 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>6</v>
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
       </c>
       <c r="E13" s="9"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="F13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="9"/>
-      <c r="F14" s="6"/>
+      <c r="F14" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -960,35 +969,37 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="8" t="s">
-        <v>32</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E16" s="9"/>
-      <c r="F16" s="6"/>
+      <c r="F16" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -996,51 +1007,61 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E17" s="9"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="8"/>
+      <c r="F17" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E18" s="9"/>
-      <c r="F18" s="6"/>
+      <c r="F18" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="12" t="s">
+      <c r="B19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="14"/>
+      <c r="D19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">

</xml_diff>

<commit_message>
Fixade php script till navbar. Ska lämna in nu :)
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92556CA-DA22-49CF-AAB7-5E89D5DE05A7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F8151D-810E-4DCD-B357-5D204B8929F3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="765" windowWidth="19440" windowHeight="15000" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
@@ -671,7 +671,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F19"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +681,7 @@
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="77.42578125" customWidth="1"/>
+    <col min="7" max="7" width="84.28515625" customWidth="1"/>
     <col min="10" max="10" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -931,15 +931,15 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="9"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="15" t="s">
         <v>37</v>
       </c>
@@ -950,13 +950,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>6</v>
+      <c r="D14" t="s">
+        <v>17</v>
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="15" t="s">
@@ -969,7 +969,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>40</v>
@@ -988,7 +988,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>40</v>
@@ -998,7 +998,7 @@
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="8"/>
     </row>
@@ -1007,31 +1007,29 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>17</v>
@@ -1040,7 +1038,9 @@
       <c r="F18" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="8"/>
+      <c r="G18" s="8" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">

</xml_diff>

<commit_message>
Råkade göra lite grejer på Sprint 3
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dropbox\Databasteknik\Hemsida\Administrativa Filer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474F5C33-92F1-470F-92A1-3C9AADBBEE2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF95CCD6-1DB9-41D3-92B1-B86D3B17054B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -638,7 +638,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,7 +1001,7 @@
       <c r="D18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="3"/>
       <c r="F18" s="10" t="s">
         <v>38</v>
       </c>
@@ -1022,7 +1022,7 @@
       <c r="D19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="3"/>
       <c r="F19" s="2" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Lite uppdateringar för inloggningen
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dropbox\Databasteknik\Hemsida\Administrativa Filer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0B064B0-92CB-4333-AA54-87A9BCA7AFA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7A0598D-2611-4F7C-BD3F-52BC142D03D5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="46">
   <si>
     <t>Uppgift</t>
   </si>
@@ -230,7 +231,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -254,17 +255,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -325,7 +315,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -333,14 +323,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
@@ -664,7 +653,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,25 +668,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>27</v>
       </c>
       <c r="J1" t="s">
@@ -933,7 +922,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>37</v>
       </c>
       <c r="G13" s="4"/>
@@ -951,8 +940,8 @@
       <c r="D14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="15"/>
-      <c r="F14" s="10" t="s">
+      <c r="E14" s="14"/>
+      <c r="F14" s="9" t="s">
         <v>37</v>
       </c>
       <c r="G14" s="4"/>
@@ -970,8 +959,8 @@
       <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="15"/>
-      <c r="F15" s="10" t="s">
+      <c r="E15" s="14"/>
+      <c r="F15" s="9" t="s">
         <v>37</v>
       </c>
       <c r="G15" s="4"/>
@@ -989,8 +978,8 @@
       <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="10" t="s">
+      <c r="E16" s="14"/>
+      <c r="F16" s="9" t="s">
         <v>37</v>
       </c>
       <c r="G16" s="4"/>
@@ -999,138 +988,140 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>6</v>
+      <c r="B17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="E17" s="15"/>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="D18" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="2" t="s">
-        <v>38</v>
+        <v>6</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="B20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="10" t="s">
+      <c r="E21" s="3"/>
+      <c r="F21" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
-        <v>20</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="9"/>
+      <c r="G21" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="B22" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="5"/>
+      <c r="F22" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="17"/>
+      <c r="E23" s="7"/>
       <c r="F23" s="10" t="s">
-        <v>37</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">

</xml_diff>

<commit_message>
Snart är köpfunktionen klar
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dropbox\Databasteknik\Hemsida\Administrativa Filer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E34A5C9-51D0-44B0-908D-06E696F7DB24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EA9992-4776-4BCF-9D5A-0B107FB0B512}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
+    <workbookView minimized="1" xWindow="2985" yWindow="1920" windowWidth="14085" windowHeight="12015" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
   <si>
     <t>Uppgift</t>
   </si>
@@ -165,10 +165,10 @@
     <t>System</t>
   </si>
   <si>
-    <t>Lägg till användare via hemsida</t>
-  </si>
-  <si>
     <t>Bara möjligheten att göra det via knappen som saknas</t>
+  </si>
+  <si>
+    <t>Möjlighet att skapa användare</t>
   </si>
 </sst>
 </file>
@@ -658,7 +658,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,7 +969,7 @@
         <v>37</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -990,7 +990,7 @@
         <v>37</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1017,21 +1017,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="15"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>47</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
@@ -1051,7 +1049,7 @@
         <v>37</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Nu kan du logga in och lägga saker i kundvagnen.
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EA9992-4776-4BCF-9D5A-0B107FB0B512}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302F70F1-147A-4C6A-B75A-D9E15184C333}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2985" yWindow="1920" windowWidth="14085" windowHeight="12015" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="49">
   <si>
     <t>Uppgift</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Möjlighet att skapa användare</t>
+  </si>
+  <si>
+    <t>Klar, typ. Man kan "köpa" en vara genom att lägga den i vagnen.</t>
   </si>
 </sst>
 </file>
@@ -658,7 +661,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,7 +993,7 @@
         <v>37</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Nu lämnar jag in sprinten
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302F70F1-147A-4C6A-B75A-D9E15184C333}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C0DA5A-8459-477E-9B9F-9D2DF8350DC3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
   <si>
     <t>Uppgift</t>
   </si>
@@ -171,7 +171,7 @@
     <t>Möjlighet att skapa användare</t>
   </si>
   <si>
-    <t>Klar, typ. Man kan "köpa" en vara genom att lägga den i vagnen.</t>
+    <t>Väldigt låg</t>
   </si>
 </sst>
 </file>
@@ -323,7 +323,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -337,7 +337,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
@@ -661,7 +660,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,13 +966,11 @@
       <c r="D15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="13"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -988,13 +985,11 @@
       <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="13"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>48</v>
-      </c>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -1009,7 +1004,7 @@
       <c r="D17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="14"/>
+      <c r="E17" s="13"/>
       <c r="F17" s="8" t="s">
         <v>37</v>
       </c>
@@ -1028,7 +1023,7 @@
       <c r="D18" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="14"/>
+      <c r="E18" s="13"/>
       <c r="F18" s="8" t="s">
         <v>37</v>
       </c>
@@ -1047,7 +1042,7 @@
       <c r="D19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="15"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="8" t="s">
         <v>37</v>
       </c>
@@ -1105,10 +1100,10 @@
         <v>41</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="8" t="s">
@@ -1127,7 +1122,7 @@
         <v>45</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="8" t="s">
@@ -1148,7 +1143,7 @@
       <c r="D24" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="16"/>
+      <c r="E24" s="15"/>
       <c r="F24" s="9" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Ändrat så sprinterna uppdateras som hänvisat
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dropbox\Databasteknik\Hemsida\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CE8C6F-2A7A-4E8A-BD8E-491736BB632B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C25147B-B61E-453D-AB8F-78A5C3A7C924}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
+    <workbookView xWindow="28680" yWindow="1500" windowWidth="29040" windowHeight="15840" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -675,7 +675,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>46</v>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>33</v>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>39</v>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G27" s="7"/>
     </row>

</xml_diff>

<commit_message>
la till en grej
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dropbox\Databasteknik\Hemsida\Administrativa Filer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C25147B-B61E-453D-AB8F-78A5C3A7C924}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0F77B0-9A3F-476F-B72A-6F1620ED88EE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1500" windowWidth="29040" windowHeight="15840" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="55">
   <si>
     <t>Uppgift</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Köpa produkt med olika antal</t>
+  </si>
+  <si>
+    <t>php $_SESSION ?</t>
   </si>
 </sst>
 </file>
@@ -338,14 +341,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -354,7 +356,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bra" xfId="1" builtinId="26"/>
@@ -675,7 +677,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="G31" sqref="G30:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,25 +692,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>27</v>
       </c>
       <c r="J1" t="s">
@@ -944,7 +946,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G13" s="4"/>
@@ -963,7 +965,7 @@
         <v>17</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G14" s="4"/>
@@ -982,7 +984,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G15" s="4"/>
@@ -1001,7 +1003,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G16" s="4"/>
@@ -1010,17 +1012,17 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="8" t="s">
+      <c r="C17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="8" t="s">
+      <c r="E17" s="12"/>
+      <c r="F17" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G17" s="4"/>
@@ -1029,17 +1031,17 @@
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="C18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="8" t="s">
+      <c r="E18" s="12"/>
+      <c r="F18" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="4"/>
@@ -1057,8 +1059,8 @@
       <c r="D19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="8" t="s">
+      <c r="E19" s="13"/>
+      <c r="F19" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G19" s="4" t="s">
@@ -1069,17 +1071,17 @@
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="8" t="s">
+      <c r="C20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G20" s="4" t="s">
@@ -1090,17 +1092,17 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="8" t="s">
+      <c r="C21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G21" s="4" t="s">
@@ -1111,19 +1113,20 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="8" t="s">
+      <c r="C22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E22" s="5"/>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="7" t="s">
         <v>38</v>
       </c>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
@@ -1139,7 +1142,7 @@
         <v>17</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="7" t="s">
         <v>37</v>
       </c>
       <c r="G23" s="4" t="s">
@@ -1171,17 +1174,17 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E25" s="5"/>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G25" s="4"/>
@@ -1190,44 +1193,58 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>48</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="15"/>
-      <c r="F27" s="9" t="s">
+      <c r="E27" s="3"/>
+      <c r="F27" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">

</xml_diff>

<commit_message>
Nu använder vi php sessioner för användarna. Inga sessionsID i länkarna
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0F77B0-9A3F-476F-B72A-6F1620ED88EE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8050FA-84E7-4596-8B66-385B27B21D7A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="56">
   <si>
     <t>Uppgift</t>
   </si>
@@ -189,7 +189,10 @@
     <t>Köpa produkt med olika antal</t>
   </si>
   <si>
-    <t>php $_SESSION ?</t>
+    <t>php sessioner</t>
+  </si>
+  <si>
+    <t>Sida för administratör</t>
   </si>
 </sst>
 </file>
@@ -356,7 +359,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bra" xfId="1" builtinId="26"/>
@@ -677,7 +680,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G31" sqref="G30:G31"/>
+      <selection activeCell="K25" sqref="K25:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,124 +1053,124 @@
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="13"/>
+      <c r="B19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="3"/>
       <c r="F19" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>46</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="7" t="s">
+      <c r="B20" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="7" t="s">
+      <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="7" t="s">
-        <v>38</v>
+      <c r="E21" s="3"/>
+      <c r="F21" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="5"/>
+      <c r="B22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="13"/>
       <c r="F22" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="4"/>
+      <c r="G22" s="4" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="B23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="5"/>
       <c r="F23" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="B24" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="2" t="s">
-        <v>37</v>
+      <c r="E24" s="5"/>
+      <c r="F24" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1175,13 +1178,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="7" t="s">
@@ -1194,7 +1197,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>45</v>
@@ -1213,43 +1216,54 @@
         <v>26</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="E27" s="5"/>
       <c r="F27" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="14"/>
-      <c r="F28" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28" s="6"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="6"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">

</xml_diff>

<commit_message>
yaay! Nu kan man lämna en recension.
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8050FA-84E7-4596-8B66-385B27B21D7A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7493AEF0-9DCC-4EEF-8C9B-38EC3730D38E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="54">
   <si>
     <t>Uppgift</t>
   </si>
@@ -165,9 +165,6 @@
     <t>System</t>
   </si>
   <si>
-    <t>Bara möjligheten att göra det via knappen som saknas</t>
-  </si>
-  <si>
     <t>Möjlighet att skapa användare</t>
   </si>
   <si>
@@ -175,9 +172,6 @@
   </si>
   <si>
     <t>Avregistrering</t>
-  </si>
-  <si>
-    <t>Än så länge kan man inte ta bort sin användare</t>
   </si>
   <si>
     <t>Möjlighet att rensa varukorgen</t>
@@ -199,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,15 +223,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,11 +239,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -338,13 +320,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -358,13 +339,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Bra" xfId="1" builtinId="26"/>
     <cellStyle name="Dålig" xfId="2" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -680,7 +659,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25:K26"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1014,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>8</v>
@@ -1123,20 +1102,18 @@
       <c r="D22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="13"/>
+      <c r="E22" s="3"/>
       <c r="F22" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>8</v>
@@ -1144,12 +1121,12 @@
       <c r="D23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="3"/>
       <c r="F23" s="7" t="s">
         <v>38</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1157,7 +1134,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>8</v>
@@ -1165,20 +1142,18 @@
       <c r="D24" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>8</v>
@@ -1186,7 +1161,7 @@
       <c r="D25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="7" t="s">
         <v>38</v>
       </c>
@@ -1203,7 +1178,7 @@
         <v>45</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="7" t="s">
@@ -1222,7 +1197,7 @@
         <v>45</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="7" t="s">
@@ -1235,7 +1210,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>8</v>
@@ -1243,7 +1218,10 @@
       <c r="D28" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1251,7 +1229,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>8</v>
@@ -1259,7 +1237,7 @@
       <c r="D29" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="14"/>
+      <c r="E29" s="13"/>
       <c r="F29" s="8" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Uppdaterat backlogen enligt våra nya förbättringar
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dropbox\Databasteknik\Hemsida\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E67E70-C190-4DB7-B681-A9C2A5DADD11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266C8C53-18FD-4AF7-946C-745800299126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
+    <workbookView xWindow="-28890" yWindow="-4905" windowWidth="19380" windowHeight="10380" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="55">
   <si>
     <t>Uppgift</t>
   </si>
@@ -144,42 +144,24 @@
     <t>S3</t>
   </si>
   <si>
-    <t>I menyn bestäms kategorier och länkar till produkterna av det som finns i databasen.</t>
-  </si>
-  <si>
     <t>Front end/databas</t>
   </si>
   <si>
-    <t>Skydd mot SQL injection</t>
-  </si>
-  <si>
     <t>Krypterade lösenord i databasen</t>
   </si>
   <si>
     <t>Byt ut alla bilder</t>
   </si>
   <si>
-    <t>Skydd mot "session hijacking"</t>
-  </si>
-  <si>
-    <t>System</t>
-  </si>
-  <si>
     <t>Möjlighet att skapa användare</t>
   </si>
   <si>
-    <t>Väldigt låg</t>
-  </si>
-  <si>
     <t>Avregistrering</t>
   </si>
   <si>
     <t>Möjlighet att rensa varukorgen</t>
   </si>
   <si>
-    <t>Det vore bra om man kan ta bort varor i varukorgen som inte finns i lager t.ex.</t>
-  </si>
-  <si>
     <t>Köpa produkt med olika antal</t>
   </si>
   <si>
@@ -187,6 +169,27 @@
   </si>
   <si>
     <t>Php sessioner</t>
+  </si>
+  <si>
+    <t>Sida för kategorier</t>
+  </si>
+  <si>
+    <t>Tömma varukorgen</t>
+  </si>
+  <si>
+    <t>Admin funktionalitet</t>
+  </si>
+  <si>
+    <t>Funktionalitet för att skilja på lagermängd</t>
+  </si>
+  <si>
+    <t>Error meddelenden</t>
+  </si>
+  <si>
+    <t>Antal varor i kundvagnen</t>
+  </si>
+  <si>
+    <t>Finslipad frontend</t>
   </si>
 </sst>
 </file>
@@ -224,7 +227,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,6 +256,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -403,12 +412,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -416,8 +423,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bra" xfId="1" builtinId="26"/>
@@ -734,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18B0A93-A15E-478B-B68F-0A6D7C63864A}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,25 +763,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>27</v>
       </c>
       <c r="J1" t="s">
@@ -779,7 +789,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -791,17 +801,17 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="12"/>
       <c r="F2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="7"/>
       <c r="J2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -813,17 +823,17 @@
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="12"/>
       <c r="F3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="7"/>
       <c r="J3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -835,14 +845,14 @@
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -854,14 +864,14 @@
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="12"/>
       <c r="F5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -873,14 +883,14 @@
       <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="12"/>
       <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -892,14 +902,14 @@
       <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="12"/>
       <c r="F7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="9"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -911,14 +921,14 @@
       <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="12"/>
       <c r="F8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="9"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -930,14 +940,14 @@
       <c r="D9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="12"/>
       <c r="F9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="9"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -949,14 +959,14 @@
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="12"/>
       <c r="F10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="9"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -968,14 +978,14 @@
       <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="9"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -987,14 +997,14 @@
       <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="12"/>
       <c r="F12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="9"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1006,128 +1016,128 @@
       <c r="D13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3" t="s">
+      <c r="E13" s="12"/>
+      <c r="F13" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="9"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3" t="s">
+      <c r="E14" s="12"/>
+      <c r="F14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="9"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3" t="s">
+      <c r="E15" s="12"/>
+      <c r="F15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="9"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="3" t="s">
+      <c r="E16" s="12"/>
+      <c r="F16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="9"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3" t="s">
+      <c r="B17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="9"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3" t="s">
+      <c r="B18" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="9"/>
+      <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
+      <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3" t="s">
+      <c r="D19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G19" s="9"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="6">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1139,16 +1149,16 @@
       <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3" t="s">
+      <c r="E20" s="12"/>
+      <c r="F20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="6">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1160,167 +1170,258 @@
       <c r="D21" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="12"/>
       <c r="F21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>39</v>
-      </c>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+      <c r="A22" s="6">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="3" t="s">
+      <c r="E22" s="12"/>
+      <c r="F22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G22" s="9"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="7"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="7"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="C26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="7"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" s="12"/>
+      <c r="F28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3" t="s">
+      <c r="E29" s="12"/>
+      <c r="F29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="G29" s="7"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
-        <v>23</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3" t="s">
+      <c r="C30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
-        <v>24</v>
-      </c>
-      <c r="B25" s="3" t="s">
+      <c r="G30" s="7"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="3" t="s">
+      <c r="C31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
-        <v>25</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3" t="s">
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
-        <v>26</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="3" t="s">
+      <c r="G32" s="7"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="8">
-        <v>27</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="3" t="s">
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="14"/>
+      <c r="F34" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10">
-        <v>28</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G29" s="13"/>
+      <c r="G34" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Vad är "Funktionalitet för att skilja på lagermängd"?
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dropbox\Databasteknik\Hemsida\Administrativa Filer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266C8C53-18FD-4AF7-946C-745800299126}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AC7713-44F9-46DF-AC05-BD6BD530370A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28890" yWindow="-4905" windowWidth="19380" windowHeight="10380" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
+    <workbookView xWindow="2985" yWindow="1920" windowWidth="14085" windowHeight="12015" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
   <si>
     <t>Uppgift</t>
   </si>
@@ -190,6 +190,24 @@
   </si>
   <si>
     <t>Finslipad frontend</t>
+  </si>
+  <si>
+    <t>Mer enhetlig design och</t>
+  </si>
+  <si>
+    <t>Alla beställningar och information om en användare ska tas bort</t>
+  </si>
+  <si>
+    <t>Möjligheten att välja antal av en vara som ska läggas i varukorgen</t>
+  </si>
+  <si>
+    <t>En sida där alla produkter inom en kategori visas som en lista.</t>
+  </si>
+  <si>
+    <t>Felmeddelanden ska ges felaktig inloggning och om recenstion läggs på ej köpt vara.</t>
+  </si>
+  <si>
+    <t>En siffra som visar hur många varor man har i kundvagnen.</t>
   </si>
 </sst>
 </file>
@@ -746,14 +764,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18B0A93-A15E-478B-B68F-0A6D7C63864A}">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
@@ -1231,7 +1249,9 @@
       <c r="F24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G24" s="7"/>
+      <c r="G24" s="7" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
@@ -1250,7 +1270,9 @@
       <c r="F25" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G25" s="7"/>
+      <c r="G25" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
@@ -1288,7 +1310,9 @@
       <c r="F27" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G27" s="7"/>
+      <c r="G27" s="7" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
@@ -1314,15 +1338,15 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="12"/>
+        <v>6</v>
+      </c>
+      <c r="E29" s="13"/>
       <c r="F29" s="2" t="s">
         <v>38</v>
       </c>
@@ -1333,15 +1357,15 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="13"/>
+        <v>17</v>
+      </c>
+      <c r="E30" s="12"/>
       <c r="F30" s="2" t="s">
         <v>38</v>
       </c>
@@ -1383,7 +1407,9 @@
       <c r="F32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="7"/>
+      <c r="G32" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
@@ -1402,7 +1428,9 @@
       <c r="F33" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G33" s="7"/>
+      <c r="G33" s="7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
@@ -1421,7 +1449,9 @@
       <c r="F34" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="10"/>
+      <c r="G34" s="10" t="s">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Du glömde avsluta kommentaren längst ner
</commit_message>
<xml_diff>
--- a/Administrativa Filer/Backlog.xlsx
+++ b/Administrativa Filer/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin\Documents\Brackets\Administrativa Filer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Dropbox\Databasteknik\Hemsida\Administrativa Filer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58AC7713-44F9-46DF-AC05-BD6BD530370A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B712A7E0-00CC-429E-8E56-9B5DFF32EC06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="1920" windowWidth="14085" windowHeight="12015" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{C3FCBA4D-8CCC-459A-932A-DF5129BA64D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -180,9 +180,6 @@
     <t>Admin funktionalitet</t>
   </si>
   <si>
-    <t>Funktionalitet för att skilja på lagermängd</t>
-  </si>
-  <si>
     <t>Error meddelenden</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>En siffra som visar hur många varor man har i kundvagnen.</t>
+  </si>
+  <si>
+    <t>Generella Klasser för knappar och formulär</t>
   </si>
 </sst>
 </file>
@@ -765,7 +765,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1250,7 +1250,7 @@
         <v>38</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1311,7 +1311,7 @@
         <v>38</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1376,10 +1376,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>14</v>
@@ -1395,7 +1395,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>8</v>
@@ -1408,7 +1408,7 @@
         <v>38</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -1416,7 +1416,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>8</v>
@@ -1429,7 +1429,7 @@
         <v>38</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1437,7 +1437,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>8</v>
@@ -1450,7 +1450,7 @@
         <v>38</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>